<commit_message>
push autosave of synergy reproducibility excel sheet
</commit_message>
<xml_diff>
--- a/synergy/reproducibility/20190812_Summary_of_Synergy_Reproducibility_Samples_Runs.xlsx
+++ b/synergy/reproducibility/20190812_Summary_of_Synergy_Reproducibility_Samples_Runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba928e3575d2bd4b/Documents/IDbyDNA/Code/AbsoluteQuantification/synergy/reproducibility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{6ECC3FB5-2F13-8643-87B9-C88FCBA13BDF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFB4673C-67BB-0E48-8789-CB4C2734574E}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{6ECC3FB5-2F13-8643-87B9-C88FCBA13BDF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8DF621B-204D-334B-8B43-0A15193DF576}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="580" windowWidth="35460" windowHeight="21020" xr2:uid="{5FB7A9A9-A8E3-B84A-B08C-98A314FCC3BA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="46760" windowHeight="21020" xr2:uid="{5FB7A9A9-A8E3-B84A-B08C-98A314FCC3BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>C19-2S1</t>
   </si>
   <si>
-    <t>Spiked urine sample C19, replicate 2 of 3 for inter-run reproducibility study, accuracy study, Candida kruesi ATCC 4247?, single urine 6, Zymo 1:10</t>
-  </si>
-  <si>
     <t>C21-2S1</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>C25-2S1</t>
   </si>
   <si>
-    <t>Spiked urine sample C25, replicate 2 of 3 for inter-run reproducibility study, replicate 1 of 4 for DNA stability study, accuracy study, Pseudominas aeruginosa, single urine 10, Zymo 1:10</t>
-  </si>
-  <si>
     <t>C26-2S1</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>C19-1S1</t>
   </si>
   <si>
-    <t>Spiked urine sample C19, replicate 1 of 3 for intra-run reproducibility study, Candida kruesi ATCC 4247?, single urine 6, Zymo 1:100</t>
-  </si>
-  <si>
     <t>C21-1S1</t>
   </si>
   <si>
@@ -180,9 +171,6 @@
     <t>C25-1S1</t>
   </si>
   <si>
-    <t>Spiked urine sample C25, replicate 1 of 3 for intra-run reproducibility study, Pseudominas aeruginosa, single urine 10, Zymo 1:100</t>
-  </si>
-  <si>
     <t>C26-1S1</t>
   </si>
   <si>
@@ -228,9 +216,6 @@
     <t>C19-2</t>
   </si>
   <si>
-    <t>Spiked urine sample C19, replicate 2 of 3 for intra-run reproducibility study, replicate 1 of 3 for inter-run reproducibility study, Candida kruesi ATCC 4247?, single urine 6, Zymo 1:100</t>
-  </si>
-  <si>
     <t>C21-2</t>
   </si>
   <si>
@@ -252,9 +237,6 @@
     <t>C25-2</t>
   </si>
   <si>
-    <t>Spiked urine sample C25, replicate 2 of 3 for intra-run reproducibility study, replicate 1 of 3 for inter-run reproducibility study, Pseudominas aeruginosa, single urine 10, Zymo 1:100</t>
-  </si>
-  <si>
     <t>C26-2</t>
   </si>
   <si>
@@ -300,9 +282,6 @@
     <t>C19-3</t>
   </si>
   <si>
-    <t>Spiked urine sample C19, replicate 3 of 3 for intra-run reproducibility study, Candida kruesi ATCC 4247?, single urine 6, Zymo 1:100</t>
-  </si>
-  <si>
     <t>C21-3</t>
   </si>
   <si>
@@ -324,9 +303,6 @@
     <t>C25-3</t>
   </si>
   <si>
-    <t>Spiked urine sample C25, replicate 3 of 3 for intra-run reproducibility study, Pseudominas aeruginosa, single urine 10, Zymo 1:100</t>
-  </si>
-  <si>
     <t>C26-3</t>
   </si>
   <si>
@@ -387,9 +363,6 @@
     <t>C25-3S2</t>
   </si>
   <si>
-    <t>Spiked urine sample C25, replicate 3 of 3 for inter-run reproducibility study, replicate 2 of 4 for DNA stability study, Pseudominas aeruginosa, single urine 10, Zymo 1:10</t>
-  </si>
-  <si>
     <t>C26-3S2</t>
   </si>
   <si>
@@ -450,9 +423,6 @@
     <t>C25-S3</t>
   </si>
   <si>
-    <t>Spiked urine sample C25, replicate 3 of 4 for DNA stability study, Pseudominas aeruginosa, single urine 10, Zymo 1:10</t>
-  </si>
-  <si>
     <t>C26-S3</t>
   </si>
   <si>
@@ -513,9 +483,6 @@
     <t>Spiked urine sample C24, replicate 4 of 4 for DNA stability study, Enterococcus faecalis, single urine 9, Zymo 1:10</t>
   </si>
   <si>
-    <t>Spiked urine sample C25, replicate 4 of 4 for DNA stability study, Pseudominas aeruginosa, single urine 10, Zymo 1:10</t>
-  </si>
-  <si>
     <t>Spiked urine sample C26, replicate 4 of 4 for DNA stability study, Escherichia coli, single urine 11, Zymo 1:10</t>
   </si>
   <si>
@@ -549,9 +516,6 @@
     <t>Candida tropicalis</t>
   </si>
   <si>
-    <t>Candida kruesi</t>
-  </si>
-  <si>
     <t>Candida parapsilosis</t>
   </si>
   <si>
@@ -561,20 +525,56 @@
     <t>Enterococcus faecalis</t>
   </si>
   <si>
-    <t>Pseudominas aeruginosa</t>
-  </si>
-  <si>
     <t>Escherichia coli</t>
   </si>
   <si>
     <t>Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t>Pichia kudriavzevii</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C19, replicate 2 of 3 for inter-run reproducibility study, accuracy study, Pichia kudriavzevii ATCC 4247?, single urine 6, Zymo 1:10</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C19, replicate 1 of 3 for intra-run reproducibility study, Pichia kudriavzevii ATCC 4247?, single urine 6, Zymo 1:100</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C19, replicate 2 of 3 for intra-run reproducibility study, replicate 1 of 3 for inter-run reproducibility study, Pichia kudriavzevii ATCC 4247?, single urine 6, Zymo 1:100</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C19, replicate 3 of 3 for intra-run reproducibility study, Pichia kudriavzevii ATCC 4247?, single urine 6, Zymo 1:100</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C25, replicate 2 of 3 for inter-run reproducibility study, replicate 1 of 4 for DNA stability study, accuracy study, Pseudomonas aeruginosa, single urine 10, Zymo 1:10</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C25, replicate 1 of 3 for intra-run reproducibility study, Pseudomonas aeruginosa, single urine 10, Zymo 1:100</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C25, replicate 2 of 3 for intra-run reproducibility study, replicate 1 of 3 for inter-run reproducibility study, Pseudomonas aeruginosa, single urine 10, Zymo 1:100</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C25, replicate 3 of 3 for intra-run reproducibility study, Pseudomonas aeruginosa, single urine 10, Zymo 1:100</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C25, replicate 3 of 3 for inter-run reproducibility study, replicate 2 of 4 for DNA stability study, Pseudomonas aeruginosa, single urine 10, Zymo 1:10</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C25, replicate 3 of 4 for DNA stability study, Pseudomonas aeruginosa, single urine 10, Zymo 1:10</t>
+  </si>
+  <si>
+    <t>Spiked urine sample C25, replicate 4 of 4 for DNA stability study, Pseudomonas aeruginosa, single urine 10, Zymo 1:10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -592,6 +592,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1108,7 +1114,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="A1:F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1132,13 +1138,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1152,13 +1158,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1172,13 +1178,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1192,13 +1198,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1212,13 +1218,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1232,13 +1238,13 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1252,13 +1258,13 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>167</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1269,16 +1275,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1289,16 +1295,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1309,16 +1315,16 @@
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1329,16 +1335,16 @@
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>171</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1349,16 +1355,16 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1369,16 +1375,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1386,19 +1392,19 @@
         <v>43690</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -1406,19 +1412,19 @@
         <v>43690</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -1426,19 +1432,19 @@
         <v>43690</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1446,19 +1452,19 @@
         <v>43690</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1466,19 +1472,19 @@
         <v>43690</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1486,19 +1492,19 @@
         <v>43690</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1506,19 +1512,19 @@
         <v>43690</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1526,19 +1532,19 @@
         <v>43690</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1546,19 +1552,19 @@
         <v>43690</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1566,19 +1572,19 @@
         <v>43690</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1586,19 +1592,19 @@
         <v>43690</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1606,19 +1612,19 @@
         <v>43690</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -1626,19 +1632,19 @@
         <v>43690</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1646,19 +1652,19 @@
         <v>43690</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -1666,19 +1672,19 @@
         <v>43690</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1686,19 +1692,19 @@
         <v>43690</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1706,19 +1712,19 @@
         <v>43690</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1726,19 +1732,19 @@
         <v>43690</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>65</v>
+        <v>169</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1746,19 +1752,19 @@
         <v>43690</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1766,19 +1772,19 @@
         <v>43690</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1786,19 +1792,19 @@
         <v>43690</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1806,19 +1812,19 @@
         <v>43690</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1826,19 +1832,19 @@
         <v>43690</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1846,19 +1852,19 @@
         <v>43690</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -1866,19 +1872,19 @@
         <v>43690</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1886,19 +1892,19 @@
         <v>43690</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -1906,19 +1912,19 @@
         <v>43690</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1926,19 +1932,19 @@
         <v>43690</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1946,19 +1952,19 @@
         <v>43690</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1966,19 +1972,19 @@
         <v>43690</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1986,19 +1992,19 @@
         <v>43690</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2006,19 +2012,19 @@
         <v>43690</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2026,19 +2032,19 @@
         <v>43690</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2046,19 +2052,19 @@
         <v>43690</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2066,19 +2072,19 @@
         <v>43690</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2086,19 +2092,19 @@
         <v>43690</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -2106,19 +2112,19 @@
         <v>43699</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2126,19 +2132,19 @@
         <v>43699</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2146,19 +2152,19 @@
         <v>43699</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2166,19 +2172,19 @@
         <v>43699</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="F53" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2186,19 +2192,19 @@
         <v>43699</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2206,19 +2212,19 @@
         <v>43699</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -2226,19 +2232,19 @@
         <v>43699</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -2246,19 +2252,19 @@
         <v>43699</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>118</v>
+        <v>176</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -2266,19 +2272,19 @@
         <v>43699</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -2286,19 +2292,19 @@
         <v>43699</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D59" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2306,19 +2312,19 @@
         <v>43700</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -2326,19 +2332,19 @@
         <v>43700</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -2346,19 +2352,19 @@
         <v>43700</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -2366,19 +2372,19 @@
         <v>43700</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2386,19 +2392,19 @@
         <v>43700</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -2406,19 +2412,19 @@
         <v>43700</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -2426,19 +2432,19 @@
         <v>43700</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -2446,19 +2452,19 @@
         <v>43700</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -2466,19 +2472,19 @@
         <v>43700</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -2486,19 +2492,19 @@
         <v>43700</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D69" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2506,19 +2512,19 @@
         <v>43701</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -2526,19 +2532,19 @@
         <v>43701</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2546,19 +2552,19 @@
         <v>43701</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2566,19 +2572,19 @@
         <v>43701</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2586,19 +2592,19 @@
         <v>43701</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2606,19 +2612,19 @@
         <v>43701</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2626,19 +2632,19 @@
         <v>43701</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2646,19 +2652,19 @@
         <v>43701</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -2666,19 +2672,19 @@
         <v>43701</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -2686,23 +2692,24 @@
         <v>43701</v>
       </c>
       <c r="B79" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C79" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="D79" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>